<commit_message>
Removing "final" to VO getters and setters.
</commit_message>
<xml_diff>
--- a/hotrod-project/docs/research/database-comparison.xlsx
+++ b/hotrod-project/docs/research/database-comparison.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="175">
   <si>
     <t xml:space="preserve">Features \ League</t>
   </si>
@@ -340,12 +340,15 @@
     <t xml:space="preserve">5. Index Optimization</t>
   </si>
   <si>
-    <t xml:space="preserve">Indexes on Expressions</t>
+    <t xml:space="preserve">Indexes on Expressions / Functional Indexes</t>
   </si>
   <si>
     <t xml:space="preserve">Yes *7</t>
   </si>
   <si>
+    <t xml:space="preserve">Since 8.0.15</t>
+  </si>
+  <si>
     <t xml:space="preserve">Indexes on Expressions with UDF</t>
   </si>
   <si>
@@ -359,6 +362,9 @@
   </si>
   <si>
     <t xml:space="preserve">Indexes on Virtual Columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since 12</t>
   </si>
   <si>
     <t xml:space="preserve">Yes *11</t>
@@ -913,8 +919,8 @@
   </sheetPr>
   <dimension ref="A1:L111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -922,10 +928,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="9.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12.5"/>
@@ -2727,7 +2734,7 @@
         <v>37</v>
       </c>
       <c r="G55" s="16" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="H55" s="15" t="s">
         <v>35</v>
@@ -2747,10 +2754,10 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C56" s="23" t="s">
         <v>37</v>
@@ -2785,7 +2792,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B57" s="16" t="s">
         <v>35</v>
@@ -2800,10 +2807,10 @@
         <v>35</v>
       </c>
       <c r="F57" s="23" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G57" s="23" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H57" s="15" t="s">
         <v>35</v>
@@ -2815,7 +2822,7 @@
         <v>35</v>
       </c>
       <c r="K57" s="23" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="L57" s="27" t="s">
         <v>37</v>
@@ -2823,7 +2830,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B58" s="16" t="s">
         <v>35</v>
@@ -2831,20 +2838,20 @@
       <c r="C58" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D58" s="24" t="s">
-        <v>37</v>
+      <c r="D58" s="15" t="s">
+        <v>114</v>
       </c>
       <c r="E58" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F58" s="16" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G58" s="16" t="s">
         <v>35</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I58" s="20" t="s">
         <v>35</v>
@@ -2861,7 +2868,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="12" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B59" s="16" t="s">
         <v>35</v>
@@ -2899,7 +2906,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="12" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B60" s="16" t="s">
         <v>35</v>
@@ -2914,10 +2921,10 @@
         <v>35</v>
       </c>
       <c r="F60" s="16" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H60" s="15" t="s">
         <v>35</v>
@@ -2934,16 +2941,16 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="12" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B61" s="16" t="s">
         <v>35</v>
       </c>
       <c r="C61" s="29" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D61" s="32" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E61" s="24" t="s">
         <v>37</v>
@@ -2969,16 +2976,16 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="31" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B62" s="23" t="s">
         <v>37</v>
       </c>
       <c r="C62" s="29" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E62" s="15" t="s">
         <v>35</v>
@@ -3004,7 +3011,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="31" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B63" s="16" t="s">
         <v>35</v>
@@ -3042,7 +3049,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>8</v>
@@ -3080,7 +3087,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="12" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B65" s="16" t="s">
         <v>35</v>
@@ -3118,7 +3125,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="12" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B66" s="16" t="s">
         <v>35</v>
@@ -3154,7 +3161,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="12" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B67" s="16" t="s">
         <v>35</v>
@@ -3163,16 +3170,16 @@
         <v>35</v>
       </c>
       <c r="D67" s="30" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E67" s="30" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F67" s="29" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G67" s="29" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H67" s="24" t="s">
         <v>37</v>
@@ -3192,40 +3199,40 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E68" s="15" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F68" s="16" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G68" s="16" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H68" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="I68" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="I68" s="20" t="s">
-        <v>132</v>
-      </c>
       <c r="J68" s="21" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K68" s="22" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L68" s="22" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3242,7 +3249,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="6" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>8</v>
@@ -3280,22 +3287,22 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C71" s="29" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E71" s="30" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F71" s="29" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G71" s="23" t="s">
         <v>20</v>
@@ -3304,13 +3311,13 @@
         <v>20</v>
       </c>
       <c r="I71" s="16" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="J71" s="29" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="K71" s="29" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3351,7 +3358,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B75" s="0"/>
       <c r="C75" s="0"/>
@@ -3366,7 +3373,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B76" s="0"/>
       <c r="C76" s="0"/>
@@ -3381,7 +3388,7 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B77" s="0"/>
       <c r="C77" s="0"/>
@@ -3396,7 +3403,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B78" s="0"/>
       <c r="C78" s="0"/>
@@ -3411,7 +3418,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B79" s="0"/>
       <c r="C79" s="0"/>
@@ -3426,7 +3433,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B80" s="0"/>
       <c r="C80" s="0"/>
@@ -3441,7 +3448,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B81" s="0"/>
       <c r="C81" s="0"/>
@@ -3456,7 +3463,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B82" s="0"/>
       <c r="C82" s="0"/>
@@ -3471,7 +3478,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B83" s="0"/>
       <c r="C83" s="0"/>
@@ -3486,7 +3493,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B84" s="0"/>
       <c r="C84" s="0"/>
@@ -3501,7 +3508,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B85" s="0"/>
       <c r="C85" s="0"/>
@@ -3516,7 +3523,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B86" s="0"/>
       <c r="C86" s="0"/>
@@ -3531,7 +3538,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B87" s="0"/>
       <c r="C87" s="0"/>
@@ -3546,7 +3553,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B88" s="0"/>
       <c r="C88" s="0"/>
@@ -3561,7 +3568,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B89" s="0"/>
       <c r="C89" s="0"/>
@@ -3576,7 +3583,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B90" s="0"/>
       <c r="C90" s="0"/>
@@ -3591,7 +3598,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B91" s="0"/>
       <c r="C91" s="0"/>
@@ -3606,7 +3613,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B92" s="0"/>
       <c r="C92" s="0"/>
@@ -3621,7 +3628,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B93" s="0"/>
       <c r="C93" s="0"/>
@@ -3636,7 +3643,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B94" s="0"/>
       <c r="C94" s="0"/>
@@ -3651,7 +3658,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B95" s="0"/>
       <c r="C95" s="0"/>
@@ -3666,7 +3673,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B96" s="0"/>
       <c r="C96" s="0"/>
@@ -3681,7 +3688,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B97" s="0"/>
       <c r="C97" s="0"/>
@@ -3696,7 +3703,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B98" s="0"/>
       <c r="C98" s="0"/>
@@ -3711,7 +3718,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B99" s="0"/>
       <c r="C99" s="0"/>
@@ -3726,7 +3733,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B100" s="0"/>
       <c r="C100" s="0"/>
@@ -3789,7 +3796,7 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="6" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B105" s="7" t="s">
         <v>8</v>
@@ -3824,42 +3831,42 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B106" s="16" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C106" s="16" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D106" s="16" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E106" s="16" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F106" s="16" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G106" s="16" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H106" s="16" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="I106" s="16" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="J106" s="16" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="K106" s="16" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B107" s="23" t="s">
         <v>37</v>
@@ -3874,10 +3881,10 @@
         <v>37</v>
       </c>
       <c r="F107" s="23" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G107" s="23" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H107" s="23" t="s">
         <v>37</v>
@@ -3894,7 +3901,7 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B108" s="23" t="s">
         <v>37</v>
@@ -3909,10 +3916,10 @@
         <v>37</v>
       </c>
       <c r="F108" s="23" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G108" s="23" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H108" s="16" t="s">
         <v>35</v>
@@ -3929,12 +3936,12 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding optimizer tests and extra docs.
</commit_message>
<xml_diff>
--- a/hotrod-project/docs/research/database-comparison.xlsx
+++ b/hotrod-project/docs/research/database-comparison.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="225">
   <si>
     <t xml:space="preserve">Features \ League</t>
   </si>
@@ -250,6 +250,9 @@
     <t xml:space="preserve">Within supported</t>
   </si>
   <si>
+    <t xml:space="preserve">Aggregation expressions, that are NOT window functions</t>
+  </si>
+  <si>
     <t xml:space="preserve">SQL:2006</t>
   </si>
   <si>
@@ -521,6 +524,153 @@
   </si>
   <si>
     <t xml:space="preserve">*26 Only "stored" generated columns are implemented. "virtual" ones are not yet implemented.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. NOT window functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">count(distinct &lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum(distinct &lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avg(distinct &lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">listagg(distinct &lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Aggregations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">count(*) / count_big</t>
+  </si>
+  <si>
+    <t xml:space="preserve">count(&lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum(&lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min(&lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max(&lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avg(&lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">listagg(&lt;expr&gt;) / string_agg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">median(&lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stddev(&lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stddev_pop(&lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stddev_samp(&lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variance(&lt;expr&gt;) / var</t>
+  </si>
+  <si>
+    <t xml:space="preserve">var_pop(&lt;expr&gt;) / varp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">var_samp(&lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">covar_pop(&lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">covar_samp(&lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">corr(&lt;expr1&gt;, &lt;expr2&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratio_to_report(&lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regr_*(&lt;expr1&gt;, &lt;expr2&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bit_and(&lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bit_or(&lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bit_xor(&lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">json_arrayagg(&lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">json_objectagg(&lt;expr&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Analytic functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">row_number()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rank()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dense_rank()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ntile()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percent_rank()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cume_dist()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first_value()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">last_value()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nth_value()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentile_cont()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentile_disc()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">last()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Positional Analytic functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lag()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lead()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">next value for</t>
   </si>
   <si>
     <t xml:space="preserve">Referential Integrity</t>
@@ -554,7 +704,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -579,6 +729,34 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -703,7 +881,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -820,6 +998,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -838,6 +1024,54 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -903,7 +1137,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -913,17 +1147,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L111"/>
+  <dimension ref="A1:L168"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J57" activeCellId="0" sqref="J57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A142" activeCellId="0" sqref="A142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.73"/>
@@ -937,7 +1171,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2084,7 +2317,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>8</v>
@@ -2122,84 +2355,37 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="B34" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="D34" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="E34" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="F34" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="G34" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="H34" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="I34" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="J34" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="K34" s="28" t="s">
-        <v>70</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B34" s="16"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="19"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I35" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J35" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K35" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L35" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="A35" s="12"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="19"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B36" s="13"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="16"/>
       <c r="C36" s="13"/>
-      <c r="D36" s="14"/>
+      <c r="D36" s="15"/>
       <c r="E36" s="14"/>
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
@@ -2209,50 +2395,23 @@
       <c r="K36" s="19"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I37" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J37" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K37" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L37" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="A37" s="12"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="19"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B38" s="13"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="16"/>
       <c r="C38" s="13"/>
-      <c r="D38" s="14"/>
+      <c r="D38" s="15"/>
       <c r="E38" s="14"/>
       <c r="F38" s="13"/>
       <c r="G38" s="13"/>
@@ -2262,49 +2421,25 @@
       <c r="K38" s="19"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B39" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="E39" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="F39" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="G39" s="28" t="s">
-        <v>69</v>
-      </c>
+      <c r="A39" s="12"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
       <c r="H39" s="14"/>
       <c r="I39" s="17"/>
       <c r="J39" s="18"/>
       <c r="K39" s="19"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B40" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="D40" s="14"/>
-      <c r="E40" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="F40" s="28" t="s">
-        <v>69</v>
-      </c>
+      <c r="A40" s="12"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="13"/>
       <c r="G40" s="13"/>
       <c r="H40" s="14"/>
       <c r="I40" s="17"/>
@@ -2312,76 +2447,94 @@
       <c r="K40" s="19"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B41" s="7" t="s">
+      <c r="A41" s="12"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="19"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C42" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D42" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E42" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="F42" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G41" s="7" t="s">
+      <c r="G42" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H41" s="8" t="s">
+      <c r="H42" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I41" s="9" t="s">
+      <c r="I42" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J41" s="10" t="s">
+      <c r="J42" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K41" s="11" t="s">
+      <c r="K42" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="L41" s="9" t="s">
+      <c r="L42" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="17"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="19"/>
-    </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="12"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="19"/>
+      <c r="A43" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="F43" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="G43" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H43" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="I43" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="J43" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="K43" s="28" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>8</v>
@@ -2419,102 +2572,67 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F45" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="G45" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="H45" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I45" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="J45" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="K45" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="L45" s="23" t="s">
-        <v>37</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="19"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B46" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C46" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E46" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="F46" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G46" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H46" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="I46" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="J46" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K46" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="L46" s="23" t="s">
-        <v>37</v>
+      <c r="A46" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J46" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K46" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L46" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B47" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F47" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="G47" s="29" t="s">
-        <v>97</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
       <c r="H47" s="14"/>
       <c r="I47" s="17"/>
       <c r="J47" s="18"/>
@@ -2522,119 +2640,100 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B48" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C48" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D48" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E48" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="F48" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G48" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H48" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="I48" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="J48" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K48" s="22" t="s">
-        <v>35</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B48" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E48" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F48" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="G48" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="H48" s="14"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="19"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="B49" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E49" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F49" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G49" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H49" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="I49" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="J49" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K49" s="27" t="s">
-        <v>37</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B49" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49" s="14"/>
+      <c r="E49" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="F49" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="G49" s="13"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="17"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="19"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="B50" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C50" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E50" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F50" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G50" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H50" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="I50" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="J50" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K50" s="27" t="s">
-        <v>37</v>
+      <c r="A50" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H50" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I50" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J50" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K50" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L50" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B51" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C51" s="16" t="s">
-        <v>35</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B51" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C51" s="13"/>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
       <c r="F51" s="13"/>
@@ -2645,12 +2744,8 @@
       <c r="K51" s="19"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B52" s="16" t="s">
-        <v>35</v>
-      </c>
+      <c r="A52" s="12"/>
+      <c r="B52" s="13"/>
       <c r="C52" s="13"/>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
@@ -2662,70 +2757,93 @@
       <c r="K52" s="19"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="B53" s="13"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="17"/>
-      <c r="J53" s="18"/>
-      <c r="K53" s="19"/>
+      <c r="A53" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I53" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J53" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K53" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L53" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F54" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H54" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I54" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J54" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K54" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L54" s="9" t="s">
-        <v>18</v>
+      <c r="A54" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E54" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F54" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="G54" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="H54" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I54" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="J54" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K54" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="L54" s="23" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="31" t="s">
-        <v>106</v>
+      <c r="A55" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="B55" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C55" s="16" t="s">
-        <v>35</v>
+      <c r="C55" s="23" t="s">
+        <v>37</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>107</v>
+        <v>35</v>
       </c>
       <c r="E55" s="24" t="s">
         <v>37</v>
@@ -2733,11 +2851,11 @@
       <c r="F55" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G55" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="H55" s="15" t="s">
-        <v>35</v>
+      <c r="G55" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H55" s="24" t="s">
+        <v>37</v>
       </c>
       <c r="I55" s="25" t="s">
         <v>37</v>
@@ -2748,89 +2866,75 @@
       <c r="K55" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="L55" s="27" t="s">
+      <c r="L55" s="23" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="12" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="C56" s="23" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>35</v>
       </c>
       <c r="D56" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E56" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="F56" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G56" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H56" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I56" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="J56" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K56" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="L56" s="27" t="s">
-        <v>37</v>
-      </c>
+      <c r="E56" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F56" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="G56" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="H56" s="14"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="18"/>
+      <c r="K56" s="19"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="12" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B57" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C57" s="16" t="s">
-        <v>35</v>
+      <c r="C57" s="23" t="s">
+        <v>37</v>
       </c>
       <c r="D57" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E57" s="15" t="s">
-        <v>35</v>
+      <c r="E57" s="24" t="s">
+        <v>37</v>
       </c>
       <c r="F57" s="23" t="s">
-        <v>112</v>
+        <v>37</v>
       </c>
       <c r="G57" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="H57" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I57" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J57" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="K57" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="L57" s="27" t="s">
-        <v>37</v>
+        <v>37</v>
+      </c>
+      <c r="H57" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I57" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="J57" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K57" s="22" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="12" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B58" s="16" t="s">
         <v>35</v>
@@ -2839,36 +2943,33 @@
         <v>35</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>114</v>
+        <v>35</v>
       </c>
       <c r="E58" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F58" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="G58" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="H58" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="I58" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J58" s="21" t="s">
-        <v>35</v>
+      <c r="F58" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G58" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H58" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I58" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J58" s="26" t="s">
+        <v>37</v>
       </c>
       <c r="K58" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="L58" s="27" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="12" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="B59" s="16" t="s">
         <v>35</v>
@@ -2888,8 +2989,8 @@
       <c r="G59" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H59" s="15" t="s">
-        <v>35</v>
+      <c r="H59" s="24" t="s">
+        <v>37</v>
       </c>
       <c r="I59" s="25" t="s">
         <v>37</v>
@@ -2899,233 +3000,176 @@
       </c>
       <c r="K59" s="27" t="s">
         <v>37</v>
-      </c>
-      <c r="L59" s="15" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="12" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="B60" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C60" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D60" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E60" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F60" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="G60" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="H60" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I60" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="J60" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K60" s="27" t="s">
-        <v>37</v>
-      </c>
+      <c r="C60" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="17"/>
+      <c r="J60" s="18"/>
+      <c r="K60" s="19"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="12" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B61" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C61" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="D61" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="E61" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="F61" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G61" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H61" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="I61" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="J61" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K61" s="27" t="s">
-        <v>37</v>
-      </c>
+      <c r="C61" s="13"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="17"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="19"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="B62" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C62" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="D62" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="E62" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F62" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G62" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H62" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="I62" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="J62" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K62" s="27" t="s">
-        <v>37</v>
-      </c>
+      <c r="A62" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B62" s="13"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="17"/>
+      <c r="J62" s="18"/>
+      <c r="K62" s="19"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="B63" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C63" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D63" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E63" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F63" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G63" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H63" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="I63" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="J63" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K63" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="L63" s="27" t="s">
-        <v>37</v>
+      <c r="A63" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H63" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I63" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J63" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K63" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L63" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E64" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F64" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G64" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H64" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I64" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J64" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K64" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L64" s="9" t="s">
-        <v>18</v>
+      <c r="A64" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E64" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F64" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G64" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H64" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I64" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J64" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K64" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="L64" s="27" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="12" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C65" s="16" t="s">
-        <v>35</v>
+        <v>111</v>
+      </c>
+      <c r="C65" s="23" t="s">
+        <v>37</v>
       </c>
       <c r="D65" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E65" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F65" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G65" s="16" t="s">
-        <v>35</v>
+      <c r="E65" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F65" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G65" s="23" t="s">
+        <v>37</v>
       </c>
       <c r="H65" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="I65" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J65" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="K65" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="L65" s="22" t="s">
-        <v>35</v>
+      <c r="I65" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J65" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K65" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="L65" s="27" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="12" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B66" s="16" t="s">
         <v>35</v>
@@ -3139,11 +3183,11 @@
       <c r="E66" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F66" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G66" s="16" t="s">
-        <v>35</v>
+      <c r="F66" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="G66" s="23" t="s">
+        <v>113</v>
       </c>
       <c r="H66" s="15" t="s">
         <v>35</v>
@@ -3151,17 +3195,19 @@
       <c r="I66" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J66" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K66" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="L66" s="19"/>
+      <c r="J66" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="K66" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="L66" s="27" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="12" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="B67" s="16" t="s">
         <v>35</v>
@@ -3169,242 +3215,404 @@
       <c r="C67" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D67" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="E67" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="F67" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="G67" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="H67" s="24" t="s">
-        <v>37</v>
+      <c r="D67" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="E67" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F67" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="G67" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H67" s="15" t="s">
+        <v>117</v>
       </c>
       <c r="I67" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K67" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="L67" s="26" t="s">
+      <c r="J67" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="K67" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="L67" s="27" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C68" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E68" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F68" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G68" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H68" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I68" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J68" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K68" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="L68" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C69" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D69" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E69" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F69" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="G69" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="H69" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I69" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J69" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K69" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C70" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="D70" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="E70" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F70" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G70" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H70" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I70" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J70" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K70" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="B71" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C71" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E71" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F71" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G71" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H71" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I71" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J71" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K71" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C72" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E72" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F72" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G72" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H72" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I72" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J72" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K72" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="L72" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H73" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I73" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J73" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K73" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L73" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C74" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E74" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F74" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G74" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H74" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I74" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J74" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="K74" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L74" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B75" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C75" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E75" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F75" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G75" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H75" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I75" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J75" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K75" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L75" s="19"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C76" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D76" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="E76" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="F76" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="B68" s="16" t="s">
+      <c r="G76" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="H76" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I76" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J76" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K76" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L76" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C68" s="16" t="s">
+      <c r="B77" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="D68" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="E68" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="F68" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="G68" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="H68" s="15" t="s">
+      <c r="C77" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="I68" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="J68" s="21" t="s">
+      <c r="D77" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="K68" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="L68" s="22" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="0"/>
-      <c r="C69" s="0"/>
-      <c r="D69" s="0"/>
-      <c r="E69" s="0"/>
-      <c r="F69" s="0"/>
-      <c r="G69" s="0"/>
-      <c r="H69" s="0"/>
-      <c r="I69" s="0"/>
-      <c r="J69" s="0"/>
-      <c r="K69" s="0"/>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="6" t="s">
+      <c r="E77" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="F77" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="G77" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="H77" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B70" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D70" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E70" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F70" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G70" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H70" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I70" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J70" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K70" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L70" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="B71" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C71" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="D71" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="E71" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="F71" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="G71" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="H71" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="I71" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="J71" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="K71" s="29" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="0"/>
-      <c r="C72" s="0"/>
-      <c r="D72" s="0"/>
-      <c r="E72" s="0"/>
-      <c r="F72" s="0"/>
-      <c r="G72" s="0"/>
-      <c r="H72" s="0"/>
-      <c r="I72" s="0"/>
-      <c r="J72" s="0"/>
-      <c r="K72" s="0"/>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="0"/>
-      <c r="C73" s="0"/>
-      <c r="D73" s="0"/>
-      <c r="E73" s="0"/>
-      <c r="F73" s="0"/>
-      <c r="G73" s="0"/>
-      <c r="H73" s="0"/>
-      <c r="I73" s="0"/>
-      <c r="J73" s="0"/>
-      <c r="K73" s="0"/>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="0"/>
-      <c r="C74" s="0"/>
-      <c r="D74" s="0"/>
-      <c r="E74" s="0"/>
-      <c r="F74" s="0"/>
-      <c r="G74" s="0"/>
-      <c r="H74" s="0"/>
-      <c r="I74" s="0"/>
-      <c r="J74" s="0"/>
-      <c r="K74" s="0"/>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="B75" s="0"/>
-      <c r="C75" s="0"/>
-      <c r="D75" s="0"/>
-      <c r="E75" s="0"/>
-      <c r="F75" s="0"/>
-      <c r="G75" s="0"/>
-      <c r="H75" s="0"/>
-      <c r="I75" s="0"/>
-      <c r="J75" s="0"/>
-      <c r="K75" s="0"/>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="B76" s="0"/>
-      <c r="C76" s="0"/>
-      <c r="D76" s="0"/>
-      <c r="E76" s="0"/>
-      <c r="F76" s="0"/>
-      <c r="G76" s="0"/>
-      <c r="H76" s="0"/>
-      <c r="I76" s="0"/>
-      <c r="J76" s="33"/>
-      <c r="K76" s="33"/>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="B77" s="0"/>
-      <c r="C77" s="0"/>
-      <c r="D77" s="0"/>
-      <c r="E77" s="0"/>
-      <c r="F77" s="0"/>
-      <c r="G77" s="0"/>
-      <c r="H77" s="0"/>
-      <c r="I77" s="0"/>
-      <c r="J77" s="0"/>
-      <c r="K77" s="0"/>
+      <c r="I77" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="J77" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="K77" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="L77" s="22" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
-        <v>144</v>
-      </c>
       <c r="B78" s="0"/>
       <c r="C78" s="0"/>
       <c r="D78" s="0"/>
@@ -3417,39 +3625,79 @@
       <c r="K78" s="0"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B79" s="0"/>
-      <c r="C79" s="0"/>
-      <c r="D79" s="0"/>
-      <c r="E79" s="0"/>
-      <c r="F79" s="0"/>
-      <c r="G79" s="0"/>
-      <c r="H79" s="0"/>
-      <c r="I79" s="0"/>
-      <c r="J79" s="0"/>
-      <c r="K79" s="0"/>
+      <c r="A79" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G79" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H79" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I79" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J79" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K79" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L79" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="B80" s="0"/>
-      <c r="C80" s="0"/>
-      <c r="D80" s="0"/>
-      <c r="E80" s="0"/>
-      <c r="F80" s="0"/>
-      <c r="G80" s="0"/>
-      <c r="H80" s="0"/>
-      <c r="I80" s="0"/>
-      <c r="J80" s="0"/>
-      <c r="K80" s="0"/>
+        <v>139</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C80" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="E80" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="F80" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="G80" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H80" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I80" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="J80" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="K80" s="31" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
-        <v>147</v>
-      </c>
       <c r="B81" s="0"/>
       <c r="C81" s="0"/>
       <c r="D81" s="0"/>
@@ -3462,9 +3710,6 @@
       <c r="K81" s="0"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
-        <v>148</v>
-      </c>
       <c r="B82" s="0"/>
       <c r="C82" s="0"/>
       <c r="D82" s="0"/>
@@ -3477,9 +3722,6 @@
       <c r="K82" s="0"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
-        <v>149</v>
-      </c>
       <c r="B83" s="0"/>
       <c r="C83" s="0"/>
       <c r="D83" s="0"/>
@@ -3493,7 +3735,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B84" s="0"/>
       <c r="C84" s="0"/>
@@ -3508,7 +3750,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B85" s="0"/>
       <c r="C85" s="0"/>
@@ -3518,12 +3760,12 @@
       <c r="G85" s="0"/>
       <c r="H85" s="0"/>
       <c r="I85" s="0"/>
-      <c r="J85" s="0"/>
-      <c r="K85" s="0"/>
+      <c r="J85" s="35"/>
+      <c r="K85" s="35"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B86" s="0"/>
       <c r="C86" s="0"/>
@@ -3538,7 +3780,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B87" s="0"/>
       <c r="C87" s="0"/>
@@ -3553,7 +3795,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B88" s="0"/>
       <c r="C88" s="0"/>
@@ -3568,7 +3810,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B89" s="0"/>
       <c r="C89" s="0"/>
@@ -3583,7 +3825,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B90" s="0"/>
       <c r="C90" s="0"/>
@@ -3598,7 +3840,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B91" s="0"/>
       <c r="C91" s="0"/>
@@ -3613,7 +3855,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B92" s="0"/>
       <c r="C92" s="0"/>
@@ -3628,7 +3870,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B93" s="0"/>
       <c r="C93" s="0"/>
@@ -3643,7 +3885,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B94" s="0"/>
       <c r="C94" s="0"/>
@@ -3658,7 +3900,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B95" s="0"/>
       <c r="C95" s="0"/>
@@ -3673,7 +3915,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B96" s="0"/>
       <c r="C96" s="0"/>
@@ -3688,7 +3930,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B97" s="0"/>
       <c r="C97" s="0"/>
@@ -3703,7 +3945,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B98" s="0"/>
       <c r="C98" s="0"/>
@@ -3718,7 +3960,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B99" s="0"/>
       <c r="C99" s="0"/>
@@ -3733,7 +3975,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B100" s="0"/>
       <c r="C100" s="0"/>
@@ -3747,6 +3989,9 @@
       <c r="K100" s="0"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>159</v>
+      </c>
       <c r="B101" s="0"/>
       <c r="C101" s="0"/>
       <c r="D101" s="0"/>
@@ -3759,6 +4004,9 @@
       <c r="K101" s="0"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>160</v>
+      </c>
       <c r="B102" s="0"/>
       <c r="C102" s="0"/>
       <c r="D102" s="0"/>
@@ -3771,6 +4019,9 @@
       <c r="K102" s="0"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>161</v>
+      </c>
       <c r="B103" s="0"/>
       <c r="C103" s="0"/>
       <c r="D103" s="0"/>
@@ -3783,6 +4034,9 @@
       <c r="K103" s="0"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>162</v>
+      </c>
       <c r="B104" s="0"/>
       <c r="C104" s="0"/>
       <c r="D104" s="0"/>
@@ -3795,153 +4049,1636 @@
       <c r="K104" s="0"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B105" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C105" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D105" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E105" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F105" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G105" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H105" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I105" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J105" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K105" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="A105" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B105" s="0"/>
+      <c r="C105" s="0"/>
+      <c r="D105" s="0"/>
+      <c r="E105" s="0"/>
+      <c r="F105" s="0"/>
+      <c r="G105" s="0"/>
+      <c r="H105" s="0"/>
+      <c r="I105" s="0"/>
+      <c r="J105" s="0"/>
+      <c r="K105" s="0"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="B106" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="C106" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="D106" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="E106" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="F106" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="G106" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="H106" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="I106" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="J106" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="K106" s="16" t="s">
-        <v>169</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="B106" s="0"/>
+      <c r="C106" s="0"/>
+      <c r="D106" s="0"/>
+      <c r="E106" s="0"/>
+      <c r="F106" s="0"/>
+      <c r="G106" s="0"/>
+      <c r="H106" s="0"/>
+      <c r="I106" s="0"/>
+      <c r="J106" s="0"/>
+      <c r="K106" s="0"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="B107" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C107" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D107" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="E107" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="F107" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="G107" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="H107" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="I107" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="J107" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="K107" s="23" t="s">
-        <v>37</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="B107" s="0"/>
+      <c r="C107" s="0"/>
+      <c r="D107" s="0"/>
+      <c r="E107" s="0"/>
+      <c r="F107" s="0"/>
+      <c r="G107" s="0"/>
+      <c r="H107" s="0"/>
+      <c r="I107" s="0"/>
+      <c r="J107" s="0"/>
+      <c r="K107" s="0"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B108" s="0"/>
+      <c r="C108" s="0"/>
+      <c r="D108" s="0"/>
+      <c r="E108" s="0"/>
+      <c r="F108" s="0"/>
+      <c r="G108" s="0"/>
+      <c r="H108" s="0"/>
+      <c r="I108" s="0"/>
+      <c r="J108" s="0"/>
+      <c r="K108" s="0"/>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B109" s="0"/>
+      <c r="C109" s="0"/>
+      <c r="D109" s="0"/>
+      <c r="E109" s="0"/>
+      <c r="F109" s="0"/>
+      <c r="G109" s="0"/>
+      <c r="H109" s="0"/>
+      <c r="I109" s="0"/>
+      <c r="J109" s="0"/>
+      <c r="K109" s="0"/>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="0"/>
+      <c r="C110" s="0"/>
+      <c r="D110" s="0"/>
+      <c r="E110" s="0"/>
+      <c r="F110" s="0"/>
+      <c r="G110" s="0"/>
+      <c r="H110" s="0"/>
+      <c r="I110" s="0"/>
+      <c r="J110" s="0"/>
+      <c r="K110" s="0"/>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B111" s="36"/>
+      <c r="C111" s="36"/>
+      <c r="D111" s="37"/>
+      <c r="E111" s="37"/>
+      <c r="F111" s="36"/>
+      <c r="G111" s="36"/>
+      <c r="H111" s="37"/>
+      <c r="I111" s="38"/>
+      <c r="J111" s="39"/>
+      <c r="K111" s="40"/>
+      <c r="L111" s="38"/>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D112" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E112" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F112" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G112" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H112" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I112" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J112" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K112" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L112" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="B113" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C113" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D113" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E113" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F113" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G113" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H113" s="14"/>
+      <c r="I113" s="17"/>
+      <c r="J113" s="18"/>
+      <c r="K113" s="19"/>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B114" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C114" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D114" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E114" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F114" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G114" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H114" s="14"/>
+      <c r="I114" s="17"/>
+      <c r="J114" s="18"/>
+      <c r="K114" s="19"/>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="B115" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C115" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D115" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E115" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F115" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G115" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H115" s="14"/>
+      <c r="I115" s="17"/>
+      <c r="J115" s="18"/>
+      <c r="K115" s="19"/>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="42" t="s">
         <v>172</v>
       </c>
-      <c r="B108" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C108" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D108" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E108" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="F108" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="G108" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="H108" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="I108" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="J108" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="K108" s="16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="s">
+      <c r="B116" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C116" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D116" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E116" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F116" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G116" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H116" s="14"/>
+      <c r="I116" s="17"/>
+      <c r="J116" s="18"/>
+      <c r="K116" s="19"/>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="41" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
+      <c r="B117" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D117" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E117" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F117" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G117" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H117" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I117" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J117" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K117" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L117" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="42" t="s">
         <v>174</v>
+      </c>
+      <c r="B118" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C118" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D118" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E118" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F118" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G118" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H118" s="14"/>
+      <c r="I118" s="17"/>
+      <c r="J118" s="18"/>
+      <c r="K118" s="19"/>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="B119" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C119" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D119" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E119" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F119" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G119" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H119" s="14"/>
+      <c r="I119" s="0"/>
+      <c r="J119" s="0"/>
+      <c r="K119" s="0"/>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="B120" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C120" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D120" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E120" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F120" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G120" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H120" s="14"/>
+      <c r="I120" s="0"/>
+      <c r="J120" s="0"/>
+      <c r="K120" s="0"/>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="B121" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C121" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D121" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E121" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F121" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G121" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H121" s="14"/>
+      <c r="I121" s="0"/>
+      <c r="J121" s="0"/>
+      <c r="K121" s="0"/>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="B122" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C122" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D122" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E122" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F122" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G122" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H122" s="14"/>
+      <c r="I122" s="0"/>
+      <c r="J122" s="0"/>
+      <c r="K122" s="0"/>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="42" t="s">
+        <v>179</v>
+      </c>
+      <c r="B123" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C123" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D123" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E123" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F123" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G123" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H123" s="14"/>
+      <c r="I123" s="0"/>
+      <c r="J123" s="0"/>
+      <c r="K123" s="0"/>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="B124" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C124" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D124" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E124" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F124" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G124" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H124" s="14"/>
+      <c r="I124" s="0"/>
+      <c r="J124" s="0"/>
+      <c r="K124" s="0"/>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="B125" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C125" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D125" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E125" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F125" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G125" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H125" s="14"/>
+      <c r="I125" s="0"/>
+      <c r="J125" s="0"/>
+      <c r="K125" s="0"/>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="B126" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C126" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D126" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E126" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F126" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G126" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H126" s="14"/>
+      <c r="I126" s="0"/>
+      <c r="J126" s="0"/>
+      <c r="K126" s="0"/>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="B127" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C127" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D127" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E127" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F127" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G127" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H127" s="14"/>
+      <c r="I127" s="0"/>
+      <c r="J127" s="0"/>
+      <c r="K127" s="0"/>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="43" t="s">
+        <v>184</v>
+      </c>
+      <c r="B128" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C128" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D128" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E128" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F128" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G128" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H128" s="14"/>
+      <c r="I128" s="0"/>
+      <c r="J128" s="0"/>
+      <c r="K128" s="0"/>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="B129" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C129" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D129" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E129" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F129" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G129" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H129" s="14"/>
+      <c r="I129" s="0"/>
+      <c r="J129" s="0"/>
+      <c r="K129" s="0"/>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="43" t="s">
+        <v>186</v>
+      </c>
+      <c r="B130" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C130" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D130" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E130" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F130" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G130" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H130" s="14"/>
+      <c r="I130" s="0"/>
+      <c r="J130" s="0"/>
+      <c r="K130" s="0"/>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="43" t="s">
+        <v>187</v>
+      </c>
+      <c r="B131" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C131" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D131" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E131" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F131" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G131" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H131" s="14"/>
+      <c r="I131" s="0"/>
+      <c r="J131" s="0"/>
+      <c r="K131" s="0"/>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="43" t="s">
+        <v>188</v>
+      </c>
+      <c r="B132" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C132" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D132" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E132" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F132" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G132" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H132" s="14"/>
+      <c r="I132" s="0"/>
+      <c r="J132" s="0"/>
+      <c r="K132" s="0"/>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="43" t="s">
+        <v>189</v>
+      </c>
+      <c r="B133" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C133" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D133" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E133" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F133" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G133" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H133" s="14"/>
+      <c r="I133" s="0"/>
+      <c r="J133" s="0"/>
+      <c r="K133" s="0"/>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="B134" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C134" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D134" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E134" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F134" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G134" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H134" s="14"/>
+      <c r="I134" s="0"/>
+      <c r="J134" s="0"/>
+      <c r="K134" s="0"/>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="B135" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C135" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D135" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E135" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F135" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G135" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H135" s="14"/>
+      <c r="I135" s="0"/>
+      <c r="J135" s="0"/>
+      <c r="K135" s="0"/>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="43" t="s">
+        <v>192</v>
+      </c>
+      <c r="B136" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C136" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D136" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E136" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F136" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G136" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H136" s="14"/>
+      <c r="I136" s="0"/>
+      <c r="J136" s="0"/>
+      <c r="K136" s="0"/>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="43" t="s">
+        <v>193</v>
+      </c>
+      <c r="B137" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C137" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D137" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E137" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F137" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G137" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H137" s="14"/>
+      <c r="I137" s="0"/>
+      <c r="J137" s="0"/>
+      <c r="K137" s="0"/>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="43" t="s">
+        <v>194</v>
+      </c>
+      <c r="B138" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C138" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D138" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E138" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F138" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G138" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H138" s="14"/>
+      <c r="I138" s="0"/>
+      <c r="J138" s="0"/>
+      <c r="K138" s="0"/>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="43" t="s">
+        <v>195</v>
+      </c>
+      <c r="B139" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C139" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D139" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E139" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F139" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G139" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H139" s="14"/>
+      <c r="I139" s="0"/>
+      <c r="J139" s="0"/>
+      <c r="K139" s="0"/>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="B140" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C140" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D140" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E140" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F140" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G140" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H140" s="14"/>
+      <c r="I140" s="0"/>
+      <c r="J140" s="0"/>
+      <c r="K140" s="0"/>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="B141" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C141" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D141" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E141" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F141" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G141" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H141" s="14"/>
+      <c r="I141" s="0"/>
+      <c r="J141" s="0"/>
+      <c r="K141" s="0"/>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C142" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D142" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E142" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F142" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G142" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H142" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I142" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J142" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K142" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L142" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="B143" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C143" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D143" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E143" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F143" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G143" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H143" s="14"/>
+      <c r="I143" s="0"/>
+      <c r="J143" s="0"/>
+      <c r="K143" s="0"/>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="42" t="s">
+        <v>200</v>
+      </c>
+      <c r="B144" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C144" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D144" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E144" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F144" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G144" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H144" s="14"/>
+      <c r="I144" s="0"/>
+      <c r="J144" s="0"/>
+      <c r="K144" s="0"/>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="42" t="s">
+        <v>201</v>
+      </c>
+      <c r="B145" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C145" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D145" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E145" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F145" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G145" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H145" s="14"/>
+      <c r="I145" s="0"/>
+      <c r="J145" s="0"/>
+      <c r="K145" s="0"/>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="42" t="s">
+        <v>202</v>
+      </c>
+      <c r="B146" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C146" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D146" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E146" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F146" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G146" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H146" s="14"/>
+      <c r="I146" s="0"/>
+      <c r="J146" s="0"/>
+      <c r="K146" s="0"/>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="45" t="s">
+        <v>203</v>
+      </c>
+      <c r="B147" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C147" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D147" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E147" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F147" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G147" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H147" s="14"/>
+      <c r="I147" s="0"/>
+      <c r="J147" s="0"/>
+      <c r="K147" s="0"/>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="45" t="s">
+        <v>204</v>
+      </c>
+      <c r="B148" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C148" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D148" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E148" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F148" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G148" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H148" s="14"/>
+      <c r="I148" s="0"/>
+      <c r="J148" s="0"/>
+      <c r="K148" s="0"/>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="45" t="s">
+        <v>205</v>
+      </c>
+      <c r="B149" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C149" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D149" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E149" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F149" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G149" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H149" s="14"/>
+      <c r="I149" s="0"/>
+      <c r="J149" s="0"/>
+      <c r="K149" s="0"/>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="45" t="s">
+        <v>206</v>
+      </c>
+      <c r="B150" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C150" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D150" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E150" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F150" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G150" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H150" s="14"/>
+      <c r="I150" s="0"/>
+      <c r="J150" s="0"/>
+      <c r="K150" s="0"/>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="45" t="s">
+        <v>207</v>
+      </c>
+      <c r="B151" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C151" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D151" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E151" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F151" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G151" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H151" s="14"/>
+      <c r="I151" s="0"/>
+      <c r="J151" s="0"/>
+      <c r="K151" s="0"/>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="46" t="s">
+        <v>208</v>
+      </c>
+      <c r="B152" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C152" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D152" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E152" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F152" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G152" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H152" s="14"/>
+      <c r="I152" s="0"/>
+      <c r="J152" s="0"/>
+      <c r="K152" s="0"/>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="B153" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C153" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D153" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E153" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F153" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G153" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H153" s="14"/>
+      <c r="I153" s="0"/>
+      <c r="J153" s="0"/>
+      <c r="K153" s="0"/>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="47" t="s">
+        <v>210</v>
+      </c>
+      <c r="B154" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C154" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D154" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E154" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F154" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G154" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H154" s="14"/>
+      <c r="I154" s="0"/>
+      <c r="J154" s="0"/>
+      <c r="K154" s="0"/>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="B155" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C155" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D155" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E155" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F155" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G155" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H155" s="14"/>
+      <c r="I155" s="0"/>
+      <c r="J155" s="0"/>
+      <c r="K155" s="0"/>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="44" t="s">
+        <v>212</v>
+      </c>
+      <c r="B156" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C156" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D156" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E156" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F156" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G156" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H156" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I156" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J156" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K156" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L156" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="42" t="s">
+        <v>213</v>
+      </c>
+      <c r="B157" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C157" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D157" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E157" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F157" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G157" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H157" s="14"/>
+      <c r="I157" s="0"/>
+      <c r="J157" s="0"/>
+      <c r="K157" s="0"/>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="42" t="s">
+        <v>214</v>
+      </c>
+      <c r="B158" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C158" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D158" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E158" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F158" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G158" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H158" s="14"/>
+      <c r="I158" s="0"/>
+      <c r="J158" s="0"/>
+      <c r="K158" s="0"/>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="44" t="s">
+        <v>215</v>
+      </c>
+      <c r="B159" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C159" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D159" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E159" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F159" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G159" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H159" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I159" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J159" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K159" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L159" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="B160" s="0"/>
+      <c r="C160" s="0"/>
+      <c r="D160" s="0"/>
+      <c r="E160" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F160" s="0"/>
+      <c r="G160" s="0"/>
+      <c r="H160" s="0"/>
+      <c r="I160" s="0"/>
+      <c r="J160" s="0"/>
+      <c r="K160" s="0"/>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B161" s="0"/>
+      <c r="C161" s="0"/>
+      <c r="D161" s="0"/>
+      <c r="E161" s="0"/>
+      <c r="F161" s="0"/>
+      <c r="G161" s="0"/>
+      <c r="H161" s="0"/>
+      <c r="I161" s="0"/>
+      <c r="J161" s="0"/>
+      <c r="K161" s="0"/>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B162" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C162" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D162" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E162" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F162" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G162" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H162" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I162" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J162" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K162" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="B163" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="C163" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="D163" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="E163" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="F163" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="G163" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="H163" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="I163" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="J163" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="K163" s="16" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="B164" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C164" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D164" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E164" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F164" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="G164" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="H164" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I164" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="J164" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="K164" s="23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="B165" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C165" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D165" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E165" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F165" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="G165" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="H165" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I165" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="J165" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="K165" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>